<commit_message>
resultat, konklusjon, tabell, ref
</commit_message>
<xml_diff>
--- a/resources/Tabell.xlsx
+++ b/resources/Tabell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobmollatt/Documents/arbeidskrav4/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDD0A04-E303-4D47-80ED-A7A2EC9EE58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F838E1A6-56E6-A54A-B200-DAA0180981C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{B27D40C2-971B-1D4B-90E8-A87916323DF3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Utvalgstørrelse inkludert til analyse</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Intention-to-treat analyse ble brukt til å undersøke protokollens effekt på antall dager til retur til idrett, og antallet re-skader, gjennom å bruke en Cox--regresjonsmodell.Kaplan-Meier metode ble brukt for å sammenligne kumulativ survival rate med tid til retur til idrett. (survival package i R, versjon 3.4.3)</t>
+  </si>
+  <si>
+    <t>Rehabiliterings-protokoll for å styrke hamstring (usual care),</t>
   </si>
 </sst>
 </file>
@@ -633,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A60C50F-4260-7C4F-A5C1-BB4D0B662943}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,7 +847,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="256" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -855,8 +858,16 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+    <row r="14" spans="1:7" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
@@ -866,6 +877,9 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
tabeller, rydding, kilder og template
</commit_message>
<xml_diff>
--- a/resources/Tabell.xlsx
+++ b/resources/Tabell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobmollatt/Documents/arbeidskrav4/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F838E1A6-56E6-A54A-B200-DAA0180981C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24792D1B-F00C-C841-B31A-1B2D1F062B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{B27D40C2-971B-1D4B-90E8-A87916323DF3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Utvalgstørrelse inkludert til analyse</t>
   </si>
@@ -69,9 +69,6 @@
     <t xml:space="preserve">Tid til retur. Tid fra skade-tidspunkt til kriterier for retur til idrett var bestått. </t>
   </si>
   <si>
-    <t xml:space="preserve">Progressiv stegvis rehabiliterings-protokoll bestående av øvelser for å styrke hamstring-muskulatur og løping. Progresjon og gjennomføring innenfor en gitt smertegrense &lt;4 på NRS.  </t>
-  </si>
-  <si>
     <t>Askling, 2013</t>
   </si>
   <si>
@@ -169,6 +166,21 @@
   </si>
   <si>
     <t>Rehabiliterings-protokoll for å styrke hamstring (usual care),</t>
+  </si>
+  <si>
+    <t>*Hamstring strain injury - hamstringsskade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Numerical rating scale </t>
+  </si>
+  <si>
+    <t>***Platelet-rich plasma</t>
+  </si>
+  <si>
+    <t>****Platelet-poor plasma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Progressiv stegvis rehabiliterings-protokoll bestående av øvelser for å styrke hamstring-muskulatur og løping. Progresjon og gjennomføring innenfor en gitt smertegrense &lt;4 på NRS**.  </t>
   </si>
 </sst>
 </file>
@@ -205,7 +217,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -277,6 +289,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -287,13 +308,73 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -304,15 +385,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -321,6 +399,42 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A60C50F-4260-7C4F-A5C1-BB4D0B662943}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,30 +762,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="103" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>36</v>
+      <c r="G1" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="205" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -690,7 +804,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="287" customHeight="1" x14ac:dyDescent="0.2">
@@ -699,7 +813,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -723,26 +837,26 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="273" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="205" thickBot="1" x14ac:dyDescent="0.25">
@@ -751,32 +865,32 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="273" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="205" thickBot="1" x14ac:dyDescent="0.25">
@@ -785,32 +899,32 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="154" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="222" thickBot="1" x14ac:dyDescent="0.25">
@@ -819,32 +933,32 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="239" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>39</v>
+      <c r="A12" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -853,7 +967,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -864,25 +978,61 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
+      <c r="A15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
+      <c r="A16" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A18:G18"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>

</xml_diff>